<commit_message>
more updates. added 2nd page. debugging in progress
</commit_message>
<xml_diff>
--- a/Scientific_Calculator_Operations.xlsx
+++ b/Scientific_Calculator_Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ECE558-EmbeddedSystemsProgramming\ECE558-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898C3D6C-7A76-4583-8715-62C9B2185058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED5192-CB3B-4B82-904F-33D362E057D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>Function Button</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>ERROR (input ≤ 0)</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>OPENS NEW SCREEN</t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +875,14 @@
         <v>33</v>
       </c>
     </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed cos sin ln log etc display issue
</commit_message>
<xml_diff>
--- a/Scientific_Calculator_Operations.xlsx
+++ b/Scientific_Calculator_Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ECE558-EmbeddedSystemsProgramming\ECE558-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61ED5192-CB3B-4B82-904F-33D362E057D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A21321-3CC6-48B1-938C-CAC4D90F9B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>cos(op1)</t>
   </si>
   <si>
-    <t>tan(op1) (May return large values for undefined cases)</t>
-  </si>
-  <si>
     <t>ERROR</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>OPENS NEW SCREEN</t>
+  </si>
+  <si>
+    <t>tan(op1)</t>
   </si>
 </sst>
 </file>
@@ -153,14 +153,14 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -175,7 +175,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -198,16 +198,155 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,370 +656,375 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="50.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="2" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>